<commit_message>
pistesyötön yksikkötesti exceleiden valintakoeoidit oli solun verran pielessä henkilötunnus pylvään lisäyksen jälkeen
</commit_message>
<xml_diff>
--- a/src/test/resources/pistesyotto/5/muplattu.xlsx
+++ b/src/test/resources/pistesyotto/5/muplattu.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="680" windowWidth="25360" windowHeight="15380"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Pistesyöttö" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -136,10 +136,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,8 +188,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -192,12 +218,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -529,72 +565,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" hidden="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" hidden="1">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A5"/>
       <c r="B5"/>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
@@ -761,95 +799,28 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="5">
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
-  <dataValidations count="22">
-    <dataValidation type="decimal" allowBlank="1" sqref="F8">
+  <dataValidations count="3">
+    <dataValidation type="decimal" allowBlank="1" sqref="F8:F14">
       <formula1>0</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G8">
+    <dataValidation type="list" allowBlank="1" sqref="E13:E14 E10:E11 G8:G14">
       <formula1>"Merkitsemättä,Osallistui,Ei osallistunut,Ei vaadita"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="F9">
-      <formula1>0</formula1>
-      <formula2>5</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G9">
-      <formula1>"Merkitsemättä,Osallistui,Ei osallistunut,Ei vaadita"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D10">
+    <dataValidation type="decimal" allowBlank="1" sqref="D13:D14 D10:D11">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E10">
-      <formula1>"Merkitsemättä,Osallistui,Ei osallistunut,Ei vaadita"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="F10">
-      <formula1>0</formula1>
-      <formula2>5</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G10">
-      <formula1>"Merkitsemättä,Osallistui,Ei osallistunut,Ei vaadita"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D11">
-      <formula1>0</formula1>
-      <formula2>100</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E11">
-      <formula1>"Merkitsemättä,Osallistui,Ei osallistunut,Ei vaadita"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="F11">
-      <formula1>0</formula1>
-      <formula2>5</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G11">
-      <formula1>"Merkitsemättä,Osallistui,Ei osallistunut,Ei vaadita"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="F12">
-      <formula1>0</formula1>
-      <formula2>5</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G12">
-      <formula1>"Merkitsemättä,Osallistui,Ei osallistunut,Ei vaadita"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D13">
-      <formula1>0</formula1>
-      <formula2>100</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E13">
-      <formula1>"Merkitsemättä,Osallistui,Ei osallistunut,Ei vaadita"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="F13">
-      <formula1>0</formula1>
-      <formula2>5</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G13">
-      <formula1>"Merkitsemättä,Osallistui,Ei osallistunut,Ei vaadita"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D14">
-      <formula1>0</formula1>
-      <formula2>100</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E14">
-      <formula1>"Merkitsemättä,Osallistui,Ei osallistunut,Ei vaadita"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="F14">
-      <formula1>0</formula1>
-      <formula2>5</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G14">
-      <formula1>"Merkitsemättä,Osallistui,Ei osallistunut,Ei vaadita"</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Pistesyötön Excelissä hetu ja pvm eri sarakkeisiin
</commit_message>
<xml_diff>
--- a/src/test/resources/pistesyotto/5/muplattu.xlsx
+++ b/src/test/resources/pistesyotto/5/muplattu.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessika/dev/oph/valintaperusteet/valintalaskentakoostepalvelu/src/test/resources/pistesyotto/5/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="680" windowWidth="25360" windowHeight="15380"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>1.2.246.562.29.173465377510</t>
   </si>
@@ -130,6 +135,9 @@
   </si>
   <si>
     <t>040489-9768</t>
+  </si>
+  <si>
+    <t>Syntymäaika</t>
   </si>
 </sst>
 </file>
@@ -201,7 +209,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -222,6 +230,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -238,6 +250,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -563,78 +580,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D8" sqref="D8:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="44.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5"/>
       <c r="B5"/>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="D6" s="7" t="s">
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -644,96 +665,99 @@
       <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="5">
+      <c r="F8" s="4"/>
+      <c r="G8" s="5">
         <v>2</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5" t="s">
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="5">
+      <c r="E10" s="5">
         <v>3</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="5">
+      <c r="G10" s="5">
         <v>2</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="5">
+      <c r="E11" s="5">
         <v>3</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="5">
+      <c r="G11" s="5">
         <v>2</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -743,14 +767,14 @@
       <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
@@ -760,20 +784,20 @@
       <c r="C13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="5">
+      <c r="E13" s="5">
         <v>3</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="5">
+      <c r="G13" s="5">
         <v>4</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -783,46 +807,41 @@
       <c r="C14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="5">
+      <c r="E14" s="5">
         <v>3</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="5">
+      <c r="G14" s="5">
         <v>1</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="decimal" allowBlank="1" sqref="F8:F14">
+    <dataValidation type="decimal" allowBlank="1" sqref="G8:G14">
       <formula1>0</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E13:E14 E10:E11 G8:G14">
+    <dataValidation type="list" allowBlank="1" sqref="F13:F14 F10:F11 H8:H14">
       <formula1>"Merkitsemättä,Osallistui,Ei osallistunut,Ei vaadita"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D13:D14 D10:D11">
+    <dataValidation type="decimal" allowBlank="1" sqref="E13:E14 E10:E11">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 'aikaleima' to excel
</commit_message>
<xml_diff>
--- a/src/test/resources/pistesyotto/5/muplattu.xlsx
+++ b/src/test/resources/pistesyotto/5/muplattu.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessika/dev/oph/valintaperusteet/valintalaskentakoostepalvelu/src/test/resources/pistesyotto/5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jussi.jartamo/iproject/GitHub/valintaperusteet/valintalaskentakoostepalvelu/src/test/resources/pistesyotto/5/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -209,7 +209,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -229,6 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -580,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -597,152 +598,130 @@
     <col min="8" max="8" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
+    <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="E5" s="1" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="1" t="s">
+      <c r="F6" s="6"/>
+      <c r="G6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E6" s="9" t="s">
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="9" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="10"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5">
-        <v>2</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5">
+        <v>2</v>
+      </c>
       <c r="H9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="5">
-        <v>3</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="5">
-        <v>2</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E11" s="5">
         <v>3</v>
@@ -759,53 +738,53 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="5">
+        <v>3</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="5">
+        <v>2</v>
+      </c>
       <c r="H12" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="5">
-        <v>3</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="5">
-        <v>4</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E14" s="5">
         <v>3</v>
@@ -814,29 +793,52 @@
         <v>24</v>
       </c>
       <c r="G14" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="5">
+        <v>3</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="decimal" allowBlank="1" sqref="G8:G14">
+    <dataValidation type="decimal" allowBlank="1" sqref="G9:G15">
       <formula1>0</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F13:F14 F10:F11 H8:H14">
+    <dataValidation type="list" allowBlank="1" sqref="F14:F15 F11:F12 H9:H15">
       <formula1>"Merkitsemättä,Osallistui,Ei osallistunut,Ei vaadita"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="E13:E14 E10:E11">
+    <dataValidation type="decimal" allowBlank="1" sqref="E14:E15 E11:E12">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>